<commit_message>
add paper title and author names to slr
</commit_message>
<xml_diff>
--- a/slr.xlsx
+++ b/slr.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-24.04\home\avula\workspaces\precise_ws\SCENE-Guidelines\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35558846-234B-44A0-B75A-506E53B40D3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{482B416A-C38C-4397-84E9-6274182945CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="17385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="295">
   <si>
     <t>DOI</t>
   </si>
@@ -822,6 +822,126 @@
   </si>
   <si>
     <t>Resilience testing in cloud is possible, cloud systems can combat fault injection successfully</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Authors</t>
+  </si>
+  <si>
+    <t>CloudStrike: Chaos Engineering for Securityand Resiliency in Cloud Infrastructure</t>
+  </si>
+  <si>
+    <t>Securing cloud-based military systems with Security Chaos Engineering and Artificial Intelligence</t>
+  </si>
+  <si>
+    <t>Infrastructure Security Checking Service Based on Chaos Engineering Method</t>
+  </si>
+  <si>
+    <t>Evaluating operational readiness using chaos engineering simulations on Kubernetes architecture in Big Data</t>
+  </si>
+  <si>
+    <t>Enhancing DevSecOps practice with Large Language Models and Security Chaos Engineering</t>
+  </si>
+  <si>
+    <t>Enhancing Operational Resilience of Critical Infrastructure Processes Through Chaos Engineering</t>
+  </si>
+  <si>
+    <t>On the Way to Automatic Exploitation of Vulnerabilities and Validation of Systems Security through Security Chaos Engineering</t>
+  </si>
+  <si>
+    <t>Measuring Resiliency of System of Systems using Chaos Engineering Experiments</t>
+  </si>
+  <si>
+    <t>On Evaluating Self-Adaptive and Self-Healing Systems using Chaos Engineering</t>
+  </si>
+  <si>
+    <t>Chaos Engineering for Resilience Assessment of Digital Twins</t>
+  </si>
+  <si>
+    <t>Chaos engineering experiments in middleware systems using targeted network degradation and automatic fault injection</t>
+  </si>
+  <si>
+    <t>Automated Generation of Configurable Cloud-Native Chaos Testbeds</t>
+  </si>
+  <si>
+    <t>Chaos Duck: A Tool for Automatic IoT Software Fault-Tolerance Analysis</t>
+  </si>
+  <si>
+    <t>CSBAuditor: Proactive Security Risk Analysis for Cloud Storage Broker Systems</t>
+  </si>
+  <si>
+    <t>Continuous auditing and threat detection in multi-cloud infrastructure</t>
+  </si>
+  <si>
+    <t>Boosting Microservice Resilience: An Evaluation of Istio’s Impact on Kubernetes Clusters Under Chaos</t>
+  </si>
+  <si>
+    <t>μ Chaos: Moving Chaos Engineering to IoT Devices</t>
+  </si>
+  <si>
+    <t>Chaos Engineering: New Approaches To Security</t>
+  </si>
+  <si>
+    <t>Continuous Resilience Testing in AWS Environments with Advanced Fault Injection Techniques</t>
+  </si>
+  <si>
+    <t>Martin Bedoya, Sara Palacios, Daniel Diaz-López, Pantaleone Nespoli, Estefania Laverde, Sebastián Suárez</t>
+  </si>
+  <si>
+    <t>Sabina Belyaeva, Yury Yanovich</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kennedy A. Torkura, Muhammad I. H. Sukmana, Feng Cheng, Christoph Meinel </t>
+  </si>
+  <si>
+    <t>Gautam Siwach, Adinarayana Haridas, Nagaraj Chinni</t>
+  </si>
+  <si>
+    <t>Martin Bedoya, Sara Palacios, Daniel Díaz‑López, Estefania Laverde, Pantaleone Nespoli</t>
+  </si>
+  <si>
+    <t>Panagiotis Dedousis, George Stergiopoulos, George Arampatzis, Dimitris Gritzalis</t>
+  </si>
+  <si>
+    <t>Sara Palacios Chavarro, Pantaleone Nespoli, Daniel Díaz‑López, Yury Niño Roa</t>
+  </si>
+  <si>
+    <t>Thomas Bailey, Patrick Marchione, Pete Swartz, Raed Salih, Michael R. Clark, Robert Denz</t>
+  </si>
+  <si>
+    <t>Moeen Ali Naqvi, Sehrish Malik, Merve Astekin, Leon Moonen</t>
+  </si>
+  <si>
+    <t>Mattia Fogli, Carlo Giannelli, Filippo Poltronieri, Cesare Stefanelli, Mauro Tortonesi</t>
+  </si>
+  <si>
+    <t>Tony Pierce, Jason Schanck, Alex Groeger, Raed Salih, Michael R. Clark</t>
+  </si>
+  <si>
+    <t>Jacopo Soldani, Antonio Brogi</t>
+  </si>
+  <si>
+    <t>Igor Zavalyshyn, Thomas Given‑Wilson, Axel Legay, Ramin Sadre, Etienne Rivière</t>
+  </si>
+  <si>
+    <t>K. A. Torkura, M. I. H. Sukmana, T. Strauss, H. Graupner, F. Cheng, C. Meinel</t>
+  </si>
+  <si>
+    <t>K. A. Torkura, M. Sukmana, F. Cheng, C. Meinel</t>
+  </si>
+  <si>
+    <t>S. Singh, C. H. Muntean, S. Gupta</t>
+  </si>
+  <si>
+    <t>Wojciech Kalka, Tomasz Szydlo</t>
+  </si>
+  <si>
+    <t>Jamie Lewis, Chenxi Wang</t>
+  </si>
+  <si>
+    <t>Durga Praveen Devi</t>
   </si>
 </sst>
 </file>
@@ -857,8 +977,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -874,10 +997,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1202,1143 +1321,1254 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T25"/>
+  <dimension ref="A1:V20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="7" max="7" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="81.125" customWidth="1"/>
-    <col min="11" max="11" width="36.625" customWidth="1"/>
-    <col min="15" max="15" width="19.25" customWidth="1"/>
-    <col min="16" max="16" width="20" customWidth="1"/>
-    <col min="17" max="17" width="18.25" customWidth="1"/>
+    <col min="1" max="1" width="36.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="106.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="89.25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="81.125" customWidth="1"/>
+    <col min="13" max="13" width="36.625" customWidth="1"/>
+    <col min="17" max="17" width="19.25" customWidth="1"/>
+    <col min="18" max="18" width="20" customWidth="1"/>
+    <col min="19" max="19" width="18.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>255</v>
+      </c>
+      <c r="C1" t="s">
+        <v>256</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>20</v>
       </c>
       <c r="B2" t="s">
+        <v>257</v>
+      </c>
+      <c r="C2" t="s">
+        <v>278</v>
+      </c>
+      <c r="D2" t="s">
         <v>21</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>22</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>23</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>24</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>25</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>26</v>
       </c>
-      <c r="H2" t="s">
+      <c r="J2" t="s">
         <v>27</v>
       </c>
-      <c r="I2" t="s">
+      <c r="K2" t="s">
         <v>28</v>
       </c>
-      <c r="J2" t="s">
+      <c r="L2" t="s">
         <v>29</v>
       </c>
-      <c r="K2" t="s">
+      <c r="M2" t="s">
         <v>236</v>
       </c>
-      <c r="L2" t="s">
+      <c r="N2" t="s">
         <v>218</v>
       </c>
-      <c r="M2" t="s">
+      <c r="O2" t="s">
         <v>202</v>
       </c>
-      <c r="N2" t="s">
+      <c r="P2" t="s">
         <v>184</v>
       </c>
-      <c r="O2" t="s">
+      <c r="Q2" t="s">
         <v>183</v>
       </c>
-      <c r="P2" t="s">
+      <c r="R2" t="s">
         <v>150</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="S2" t="s">
         <v>31</v>
       </c>
-      <c r="R2" t="s">
+      <c r="T2" t="s">
         <v>32</v>
       </c>
-      <c r="S2" t="s">
+      <c r="U2" t="s">
         <v>33</v>
       </c>
-      <c r="T2" t="s">
+      <c r="V2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>34</v>
       </c>
       <c r="B3" t="s">
+        <v>258</v>
+      </c>
+      <c r="C3" t="s">
+        <v>276</v>
+      </c>
+      <c r="D3" t="s">
         <v>35</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
         <v>22</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
         <v>23</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
         <v>36</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H3" t="s">
         <v>25</v>
       </c>
-      <c r="G3" t="s">
+      <c r="I3" t="s">
         <v>37</v>
       </c>
-      <c r="H3" t="s">
+      <c r="J3" t="s">
         <v>38</v>
       </c>
-      <c r="I3" t="s">
+      <c r="K3" t="s">
         <v>28</v>
       </c>
-      <c r="J3" t="s">
+      <c r="L3" t="s">
         <v>39</v>
       </c>
-      <c r="K3" t="s">
+      <c r="M3" t="s">
         <v>237</v>
       </c>
-      <c r="L3" t="s">
+      <c r="N3" t="s">
         <v>219</v>
       </c>
-      <c r="M3" t="s">
+      <c r="O3" t="s">
         <v>203</v>
       </c>
-      <c r="N3" t="s">
+      <c r="P3" t="s">
         <v>185</v>
       </c>
-      <c r="O3" t="s">
+      <c r="Q3" t="s">
         <v>179</v>
       </c>
-      <c r="P3" t="s">
+      <c r="R3" t="s">
         <v>151</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="S3" t="s">
         <v>40</v>
       </c>
-      <c r="R3" t="s">
+      <c r="T3" t="s">
         <v>41</v>
       </c>
-      <c r="S3" t="s">
+      <c r="U3" t="s">
         <v>42</v>
       </c>
-      <c r="T3" t="s">
+      <c r="V3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>43</v>
       </c>
       <c r="B4" t="s">
+        <v>259</v>
+      </c>
+      <c r="C4" t="s">
+        <v>277</v>
+      </c>
+      <c r="D4" t="s">
         <v>35</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E4" t="s">
         <v>44</v>
       </c>
-      <c r="D4" t="s">
+      <c r="F4" t="s">
         <v>23</v>
       </c>
-      <c r="E4" t="s">
+      <c r="G4" t="s">
         <v>24</v>
       </c>
-      <c r="F4" t="s">
+      <c r="H4" t="s">
         <v>25</v>
       </c>
-      <c r="G4" t="s">
+      <c r="I4" t="s">
         <v>45</v>
       </c>
-      <c r="H4" t="s">
-        <v>30</v>
-      </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
+        <v>30</v>
+      </c>
+      <c r="K4" t="s">
         <v>28</v>
       </c>
-      <c r="J4" t="s">
+      <c r="L4" t="s">
         <v>46</v>
       </c>
-      <c r="K4" t="s">
+      <c r="M4" t="s">
         <v>238</v>
       </c>
-      <c r="L4" t="s">
+      <c r="N4" t="s">
         <v>220</v>
       </c>
-      <c r="M4" t="s">
+      <c r="O4" t="s">
         <v>204</v>
       </c>
-      <c r="N4" t="s">
+      <c r="P4" t="s">
         <v>186</v>
       </c>
-      <c r="O4" t="s">
+      <c r="Q4" t="s">
         <v>168</v>
       </c>
-      <c r="P4" t="s">
+      <c r="R4" t="s">
         <v>152</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="S4" t="s">
         <v>47</v>
       </c>
-      <c r="R4" t="s">
+      <c r="T4" t="s">
         <v>48</v>
       </c>
-      <c r="S4" t="s">
+      <c r="U4" t="s">
         <v>49</v>
       </c>
-      <c r="T4" t="s">
+      <c r="V4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>50</v>
       </c>
       <c r="B5" t="s">
+        <v>260</v>
+      </c>
+      <c r="C5" t="s">
+        <v>279</v>
+      </c>
+      <c r="D5" t="s">
         <v>51</v>
       </c>
-      <c r="C5" t="s">
+      <c r="E5" t="s">
         <v>22</v>
       </c>
-      <c r="D5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" t="s">
         <v>24</v>
       </c>
-      <c r="F5" t="s">
+      <c r="H5" t="s">
         <v>52</v>
       </c>
-      <c r="G5" t="s">
-        <v>30</v>
-      </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
+        <v>30</v>
+      </c>
+      <c r="J5" t="s">
         <v>53</v>
       </c>
-      <c r="I5" t="s">
-        <v>30</v>
-      </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
+        <v>30</v>
+      </c>
+      <c r="L5" t="s">
         <v>54</v>
       </c>
-      <c r="K5" t="s">
+      <c r="M5" t="s">
         <v>239</v>
       </c>
-      <c r="L5" t="s">
+      <c r="N5" t="s">
         <v>221</v>
       </c>
-      <c r="N5" t="s">
+      <c r="P5" t="s">
         <v>187</v>
       </c>
-      <c r="O5" t="s">
+      <c r="Q5" t="s">
         <v>169</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="S5" t="s">
         <v>55</v>
       </c>
-      <c r="R5" t="s">
+      <c r="T5" t="s">
         <v>56</v>
       </c>
-      <c r="S5" t="s">
+      <c r="U5" t="s">
         <v>56</v>
       </c>
-      <c r="T5" t="s">
+      <c r="V5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>57</v>
       </c>
       <c r="B6" t="s">
+        <v>261</v>
+      </c>
+      <c r="C6" t="s">
+        <v>280</v>
+      </c>
+      <c r="D6" t="s">
         <v>58</v>
       </c>
-      <c r="C6" t="s">
+      <c r="E6" t="s">
         <v>44</v>
       </c>
-      <c r="D6" t="s">
+      <c r="F6" t="s">
         <v>23</v>
       </c>
-      <c r="E6" t="s">
+      <c r="G6" t="s">
         <v>36</v>
       </c>
-      <c r="F6" t="s">
+      <c r="H6" t="s">
         <v>25</v>
       </c>
-      <c r="G6" t="s">
+      <c r="I6" t="s">
         <v>59</v>
       </c>
-      <c r="H6" t="s">
+      <c r="J6" t="s">
         <v>60</v>
       </c>
-      <c r="I6" t="s">
-        <v>30</v>
-      </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
+        <v>30</v>
+      </c>
+      <c r="L6" t="s">
         <v>39</v>
       </c>
-      <c r="K6" t="s">
+      <c r="M6" t="s">
         <v>240</v>
       </c>
-      <c r="L6" t="s">
+      <c r="N6" t="s">
         <v>222</v>
       </c>
-      <c r="M6" t="s">
+      <c r="O6" t="s">
         <v>205</v>
       </c>
-      <c r="N6" t="s">
+      <c r="P6" t="s">
         <v>188</v>
       </c>
-      <c r="O6" t="s">
+      <c r="Q6" t="s">
         <v>170</v>
       </c>
-      <c r="P6" t="s">
+      <c r="R6" t="s">
         <v>153</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="S6" t="s">
         <v>61</v>
       </c>
-      <c r="R6" t="s">
+      <c r="T6" t="s">
         <v>61</v>
       </c>
-      <c r="S6" t="s">
+      <c r="U6" t="s">
         <v>62</v>
       </c>
-      <c r="T6" t="s">
+      <c r="V6" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>63</v>
       </c>
       <c r="B7" t="s">
+        <v>262</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="D7" t="s">
         <v>35</v>
       </c>
-      <c r="C7" t="s">
+      <c r="E7" t="s">
         <v>64</v>
       </c>
-      <c r="D7" t="s">
+      <c r="F7" t="s">
         <v>23</v>
       </c>
-      <c r="E7" t="s">
+      <c r="G7" t="s">
         <v>24</v>
       </c>
-      <c r="F7" t="s">
+      <c r="H7" t="s">
         <v>52</v>
       </c>
-      <c r="G7" t="s">
-        <v>30</v>
-      </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
+        <v>30</v>
+      </c>
+      <c r="J7" t="s">
         <v>65</v>
       </c>
-      <c r="I7" t="s">
+      <c r="K7" t="s">
         <v>28</v>
       </c>
-      <c r="J7" t="s">
+      <c r="L7" t="s">
         <v>66</v>
       </c>
-      <c r="K7" t="s">
+      <c r="M7" t="s">
         <v>241</v>
       </c>
-      <c r="L7" t="s">
+      <c r="N7" t="s">
         <v>223</v>
       </c>
-      <c r="M7" t="s">
+      <c r="O7" t="s">
         <v>206</v>
       </c>
-      <c r="N7" t="s">
+      <c r="P7" t="s">
         <v>189</v>
       </c>
-      <c r="P7" t="s">
+      <c r="R7" t="s">
         <v>154</v>
       </c>
-      <c r="Q7" t="s">
+      <c r="S7" t="s">
         <v>67</v>
       </c>
-      <c r="R7" t="s">
+      <c r="T7" t="s">
         <v>68</v>
       </c>
-      <c r="S7" t="s">
+      <c r="U7" t="s">
         <v>69</v>
       </c>
-      <c r="T7" t="s">
+      <c r="V7" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>70</v>
       </c>
       <c r="B8" t="s">
+        <v>263</v>
+      </c>
+      <c r="C8" t="s">
+        <v>282</v>
+      </c>
+      <c r="D8" t="s">
         <v>35</v>
       </c>
-      <c r="C8" t="s">
+      <c r="E8" t="s">
         <v>44</v>
       </c>
-      <c r="D8" t="s">
+      <c r="F8" t="s">
         <v>23</v>
       </c>
-      <c r="E8" t="s">
+      <c r="G8" t="s">
         <v>24</v>
       </c>
-      <c r="F8" t="s">
+      <c r="H8" t="s">
         <v>71</v>
       </c>
-      <c r="G8" t="s">
+      <c r="I8" t="s">
         <v>72</v>
       </c>
-      <c r="H8" t="s">
-        <v>30</v>
-      </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
+        <v>30</v>
+      </c>
+      <c r="K8" t="s">
         <v>28</v>
       </c>
-      <c r="J8" t="s">
+      <c r="L8" t="s">
         <v>73</v>
       </c>
-      <c r="K8" t="s">
+      <c r="M8" t="s">
         <v>242</v>
       </c>
-      <c r="L8" t="s">
+      <c r="N8" t="s">
         <v>224</v>
       </c>
-      <c r="M8" t="s">
+      <c r="O8" t="s">
         <v>207</v>
       </c>
-      <c r="N8" t="s">
+      <c r="P8" t="s">
         <v>190</v>
       </c>
-      <c r="P8" t="s">
+      <c r="R8" t="s">
         <v>155</v>
       </c>
-      <c r="Q8" t="s">
+      <c r="S8" t="s">
         <v>74</v>
       </c>
-      <c r="R8" t="s">
+      <c r="T8" t="s">
         <v>75</v>
       </c>
-      <c r="S8" t="s">
+      <c r="U8" t="s">
         <v>76</v>
       </c>
-      <c r="T8" t="s">
+      <c r="V8" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>77</v>
       </c>
       <c r="B9" t="s">
+        <v>264</v>
+      </c>
+      <c r="C9" t="s">
+        <v>283</v>
+      </c>
+      <c r="D9" t="s">
         <v>51</v>
       </c>
-      <c r="C9" t="s">
+      <c r="E9" t="s">
         <v>78</v>
       </c>
-      <c r="D9" t="s">
+      <c r="F9" t="s">
         <v>79</v>
       </c>
-      <c r="E9" t="s">
+      <c r="G9" t="s">
         <v>24</v>
       </c>
-      <c r="F9" t="s">
+      <c r="H9" t="s">
         <v>52</v>
       </c>
-      <c r="G9" t="s">
+      <c r="I9" t="s">
         <v>72</v>
       </c>
-      <c r="H9" t="s">
+      <c r="J9" t="s">
         <v>80</v>
       </c>
-      <c r="I9" t="s">
+      <c r="K9" t="s">
         <v>28</v>
       </c>
-      <c r="J9" t="s">
+      <c r="L9" t="s">
         <v>81</v>
       </c>
-      <c r="K9" t="s">
+      <c r="M9" t="s">
         <v>243</v>
       </c>
-      <c r="L9" t="s">
+      <c r="N9" t="s">
         <v>225</v>
       </c>
-      <c r="M9" t="s">
+      <c r="O9" t="s">
         <v>208</v>
       </c>
-      <c r="N9" t="s">
+      <c r="P9" t="s">
         <v>191</v>
       </c>
-      <c r="O9" t="s">
+      <c r="Q9" t="s">
         <v>180</v>
       </c>
-      <c r="P9" t="s">
+      <c r="R9" t="s">
         <v>156</v>
       </c>
-      <c r="Q9" t="s">
+      <c r="S9" t="s">
         <v>82</v>
       </c>
-      <c r="R9" t="s">
+      <c r="T9" t="s">
         <v>83</v>
       </c>
-      <c r="S9" t="s">
+      <c r="U9" t="s">
         <v>84</v>
       </c>
-      <c r="T9" t="s">
+      <c r="V9" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>85</v>
       </c>
       <c r="B10" t="s">
+        <v>265</v>
+      </c>
+      <c r="C10" t="s">
+        <v>284</v>
+      </c>
+      <c r="D10" t="s">
         <v>51</v>
       </c>
-      <c r="C10" t="s">
+      <c r="E10" t="s">
         <v>44</v>
       </c>
-      <c r="D10" t="s">
+      <c r="F10" t="s">
         <v>79</v>
       </c>
-      <c r="E10" t="s">
+      <c r="G10" t="s">
         <v>24</v>
       </c>
-      <c r="F10" t="s">
+      <c r="H10" t="s">
         <v>52</v>
       </c>
-      <c r="G10" t="s">
+      <c r="I10" t="s">
         <v>86</v>
       </c>
-      <c r="H10" t="s">
+      <c r="J10" t="s">
         <v>87</v>
       </c>
-      <c r="I10" t="s">
+      <c r="K10" t="s">
         <v>28</v>
       </c>
-      <c r="J10" t="s">
+      <c r="L10" t="s">
         <v>88</v>
       </c>
-      <c r="K10" t="s">
+      <c r="M10" t="s">
         <v>244</v>
       </c>
-      <c r="L10" t="s">
+      <c r="N10" t="s">
         <v>226</v>
       </c>
-      <c r="M10" t="s">
+      <c r="O10" t="s">
         <v>209</v>
       </c>
-      <c r="N10" t="s">
+      <c r="P10" t="s">
         <v>192</v>
       </c>
-      <c r="O10" t="s">
+      <c r="Q10" t="s">
         <v>181</v>
       </c>
-      <c r="P10" t="s">
+      <c r="R10" t="s">
         <v>157</v>
       </c>
-      <c r="Q10" t="s">
+      <c r="S10" t="s">
         <v>89</v>
       </c>
-      <c r="R10" t="s">
+      <c r="T10" t="s">
         <v>90</v>
       </c>
-      <c r="S10" t="s">
+      <c r="U10" t="s">
         <v>91</v>
       </c>
-      <c r="T10" t="s">
+      <c r="V10" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>92</v>
       </c>
       <c r="B11" t="s">
+        <v>266</v>
+      </c>
+      <c r="C11" t="s">
+        <v>285</v>
+      </c>
+      <c r="D11" t="s">
         <v>58</v>
       </c>
-      <c r="C11" t="s">
+      <c r="E11" t="s">
         <v>93</v>
       </c>
-      <c r="D11" t="s">
+      <c r="F11" t="s">
         <v>23</v>
       </c>
-      <c r="E11" t="s">
+      <c r="G11" t="s">
         <v>24</v>
       </c>
-      <c r="F11" t="s">
+      <c r="H11" t="s">
         <v>25</v>
       </c>
-      <c r="G11" t="s">
-        <v>30</v>
-      </c>
-      <c r="H11" t="s">
+      <c r="I11" t="s">
+        <v>30</v>
+      </c>
+      <c r="J11" t="s">
         <v>94</v>
       </c>
-      <c r="I11" t="s">
+      <c r="K11" t="s">
         <v>28</v>
       </c>
-      <c r="J11" t="s">
+      <c r="L11" t="s">
         <v>95</v>
       </c>
-      <c r="K11" t="s">
+      <c r="M11" t="s">
         <v>245</v>
       </c>
-      <c r="L11" t="s">
+      <c r="N11" t="s">
         <v>227</v>
       </c>
-      <c r="M11" t="s">
+      <c r="O11" t="s">
         <v>210</v>
       </c>
-      <c r="N11" t="s">
+      <c r="P11" t="s">
         <v>193</v>
       </c>
-      <c r="O11" t="s">
+      <c r="Q11" t="s">
         <v>171</v>
       </c>
-      <c r="P11" t="s">
+      <c r="R11" t="s">
         <v>166</v>
       </c>
-      <c r="Q11" t="s">
+      <c r="S11" t="s">
         <v>96</v>
       </c>
-      <c r="R11" t="s">
+      <c r="T11" t="s">
         <v>97</v>
       </c>
-      <c r="S11" t="s">
+      <c r="U11" t="s">
         <v>98</v>
       </c>
-      <c r="T11" t="s">
+      <c r="V11" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>99</v>
       </c>
       <c r="B12" t="s">
+        <v>267</v>
+      </c>
+      <c r="C12" t="s">
+        <v>286</v>
+      </c>
+      <c r="D12" t="s">
         <v>100</v>
       </c>
-      <c r="C12" t="s">
+      <c r="E12" t="s">
         <v>101</v>
       </c>
-      <c r="D12" t="s">
+      <c r="F12" t="s">
         <v>79</v>
       </c>
-      <c r="E12" t="s">
+      <c r="G12" t="s">
         <v>24</v>
       </c>
-      <c r="F12" t="s">
+      <c r="H12" t="s">
         <v>52</v>
       </c>
-      <c r="G12" t="s">
-        <v>30</v>
-      </c>
-      <c r="H12" t="s">
+      <c r="I12" t="s">
+        <v>30</v>
+      </c>
+      <c r="J12" t="s">
         <v>102</v>
       </c>
-      <c r="I12" t="s">
+      <c r="K12" t="s">
         <v>28</v>
       </c>
-      <c r="J12" t="s">
+      <c r="L12" t="s">
         <v>103</v>
       </c>
-      <c r="K12" t="s">
+      <c r="M12" t="s">
         <v>246</v>
       </c>
-      <c r="L12" t="s">
+      <c r="N12" t="s">
         <v>228</v>
       </c>
-      <c r="M12" t="s">
+      <c r="O12" t="s">
         <v>211</v>
       </c>
-      <c r="N12" t="s">
+      <c r="P12" t="s">
         <v>194</v>
       </c>
-      <c r="O12" t="s">
+      <c r="Q12" t="s">
         <v>172</v>
       </c>
-      <c r="P12" t="s">
+      <c r="R12" t="s">
         <v>158</v>
       </c>
-      <c r="Q12" t="s">
+      <c r="S12" t="s">
         <v>104</v>
       </c>
-      <c r="R12" t="s">
+      <c r="T12" t="s">
         <v>105</v>
       </c>
-      <c r="S12" t="s">
+      <c r="U12" t="s">
         <v>106</v>
       </c>
-      <c r="T12" t="s">
+      <c r="V12" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>107</v>
       </c>
       <c r="B13" t="s">
+        <v>268</v>
+      </c>
+      <c r="C13" t="s">
+        <v>287</v>
+      </c>
+      <c r="D13" t="s">
         <v>100</v>
       </c>
-      <c r="C13" t="s">
+      <c r="E13" t="s">
         <v>22</v>
       </c>
-      <c r="D13" t="s">
+      <c r="F13" t="s">
         <v>79</v>
       </c>
-      <c r="E13" t="s">
+      <c r="G13" t="s">
         <v>24</v>
       </c>
-      <c r="F13" t="s">
+      <c r="H13" t="s">
         <v>52</v>
       </c>
-      <c r="G13" t="s">
-        <v>30</v>
-      </c>
-      <c r="H13" t="s">
+      <c r="I13" t="s">
+        <v>30</v>
+      </c>
+      <c r="J13" t="s">
         <v>108</v>
       </c>
-      <c r="I13" t="s">
-        <v>30</v>
-      </c>
-      <c r="J13" t="s">
+      <c r="K13" t="s">
+        <v>30</v>
+      </c>
+      <c r="L13" t="s">
         <v>109</v>
       </c>
-      <c r="K13" t="s">
+      <c r="M13" t="s">
         <v>247</v>
       </c>
-      <c r="L13" t="s">
+      <c r="N13" t="s">
         <v>229</v>
       </c>
-      <c r="M13" t="s">
+      <c r="O13" t="s">
         <v>212</v>
       </c>
-      <c r="N13" t="s">
+      <c r="P13" t="s">
         <v>195</v>
       </c>
-      <c r="O13" t="s">
+      <c r="Q13" t="s">
         <v>173</v>
       </c>
-      <c r="P13" t="s">
+      <c r="R13" t="s">
         <v>159</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>110</v>
-      </c>
-      <c r="R13" t="s">
-        <v>110</v>
       </c>
       <c r="S13" t="s">
         <v>110</v>
       </c>
       <c r="T13" t="s">
+        <v>110</v>
+      </c>
+      <c r="U13" t="s">
+        <v>110</v>
+      </c>
+      <c r="V13" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>111</v>
       </c>
       <c r="B14" t="s">
+        <v>269</v>
+      </c>
+      <c r="C14" t="s">
+        <v>288</v>
+      </c>
+      <c r="D14" t="s">
         <v>100</v>
       </c>
-      <c r="C14" t="s">
+      <c r="E14" t="s">
         <v>112</v>
       </c>
-      <c r="D14" t="s">
+      <c r="F14" t="s">
         <v>23</v>
       </c>
-      <c r="E14" t="s">
+      <c r="G14" t="s">
         <v>24</v>
       </c>
-      <c r="F14" t="s">
+      <c r="H14" t="s">
         <v>52</v>
       </c>
-      <c r="G14" t="s">
-        <v>30</v>
-      </c>
-      <c r="H14" t="s">
+      <c r="I14" t="s">
+        <v>30</v>
+      </c>
+      <c r="J14" t="s">
         <v>108</v>
       </c>
-      <c r="I14" t="s">
+      <c r="K14" t="s">
         <v>28</v>
       </c>
-      <c r="J14" t="s">
+      <c r="L14" t="s">
         <v>113</v>
       </c>
-      <c r="K14" t="s">
+      <c r="M14" t="s">
         <v>248</v>
       </c>
-      <c r="L14" t="s">
+      <c r="N14" t="s">
         <v>230</v>
       </c>
-      <c r="M14" t="s">
+      <c r="O14" t="s">
         <v>213</v>
       </c>
-      <c r="N14" t="s">
+      <c r="P14" t="s">
         <v>196</v>
       </c>
-      <c r="O14" t="s">
+      <c r="Q14" t="s">
         <v>174</v>
       </c>
-      <c r="P14" t="s">
+      <c r="R14" t="s">
         <v>160</v>
       </c>
-      <c r="Q14" t="s">
+      <c r="S14" t="s">
         <v>114</v>
       </c>
-      <c r="R14" t="s">
+      <c r="T14" t="s">
         <v>115</v>
       </c>
-      <c r="S14" t="s">
+      <c r="U14" t="s">
         <v>116</v>
       </c>
-      <c r="T14" t="s">
+      <c r="V14" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>117</v>
       </c>
       <c r="B15" t="s">
+        <v>270</v>
+      </c>
+      <c r="C15" t="s">
+        <v>289</v>
+      </c>
+      <c r="D15" t="s">
         <v>118</v>
       </c>
-      <c r="C15" t="s">
+      <c r="E15" t="s">
         <v>22</v>
       </c>
-      <c r="D15" t="s">
+      <c r="F15" t="s">
         <v>23</v>
       </c>
-      <c r="E15" t="s">
+      <c r="G15" t="s">
         <v>24</v>
       </c>
-      <c r="F15" t="s">
+      <c r="H15" t="s">
         <v>52</v>
       </c>
-      <c r="G15" t="s">
-        <v>30</v>
-      </c>
-      <c r="H15" t="s">
+      <c r="I15" t="s">
+        <v>30</v>
+      </c>
+      <c r="J15" t="s">
         <v>119</v>
       </c>
-      <c r="I15" t="s">
+      <c r="K15" t="s">
         <v>120</v>
       </c>
-      <c r="J15" t="s">
+      <c r="L15" t="s">
         <v>121</v>
       </c>
-      <c r="K15" t="s">
+      <c r="M15" t="s">
         <v>249</v>
       </c>
-      <c r="L15" t="s">
+      <c r="N15" t="s">
         <v>231</v>
       </c>
-      <c r="M15" t="s">
+      <c r="O15" t="s">
         <v>214</v>
       </c>
-      <c r="N15" t="s">
+      <c r="P15" t="s">
         <v>197</v>
       </c>
-      <c r="O15" t="s">
+      <c r="Q15" t="s">
         <v>175</v>
       </c>
-      <c r="P15" t="s">
+      <c r="R15" t="s">
         <v>161</v>
       </c>
-      <c r="Q15" t="s">
+      <c r="S15" t="s">
         <v>122</v>
       </c>
-      <c r="R15" t="s">
+      <c r="T15" t="s">
         <v>123</v>
       </c>
-      <c r="S15" t="s">
+      <c r="U15" t="s">
         <v>124</v>
       </c>
-      <c r="T15" t="s">
+      <c r="V15" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>125</v>
       </c>
       <c r="B16" t="s">
+        <v>271</v>
+      </c>
+      <c r="C16" t="s">
+        <v>290</v>
+      </c>
+      <c r="D16" t="s">
         <v>100</v>
       </c>
-      <c r="C16" t="s">
+      <c r="E16" t="s">
         <v>22</v>
       </c>
-      <c r="D16" t="s">
+      <c r="F16" t="s">
         <v>23</v>
       </c>
-      <c r="E16" t="s">
+      <c r="G16" t="s">
         <v>24</v>
       </c>
-      <c r="F16" t="s">
+      <c r="H16" t="s">
         <v>126</v>
       </c>
-      <c r="G16" t="s">
-        <v>30</v>
-      </c>
-      <c r="H16" t="s">
+      <c r="I16" t="s">
+        <v>30</v>
+      </c>
+      <c r="J16" t="s">
         <v>127</v>
       </c>
-      <c r="I16" t="s">
+      <c r="K16" t="s">
         <v>28</v>
       </c>
-      <c r="J16" t="s">
+      <c r="L16" t="s">
         <v>128</v>
       </c>
-      <c r="K16" t="s">
+      <c r="M16" t="s">
         <v>250</v>
       </c>
-      <c r="L16" t="s">
+      <c r="N16" t="s">
         <v>232</v>
       </c>
-      <c r="M16" t="s">
+      <c r="O16" t="s">
         <v>215</v>
       </c>
-      <c r="N16" t="s">
+      <c r="P16" t="s">
         <v>198</v>
       </c>
-      <c r="O16" t="s">
+      <c r="Q16" t="s">
         <v>176</v>
       </c>
-      <c r="P16" t="s">
+      <c r="R16" t="s">
         <v>162</v>
       </c>
-      <c r="Q16" t="s">
+      <c r="S16" t="s">
         <v>129</v>
       </c>
-      <c r="R16" t="s">
+      <c r="T16" t="s">
         <v>130</v>
       </c>
-      <c r="S16" t="s">
+      <c r="U16" t="s">
         <v>131</v>
       </c>
-      <c r="T16" t="s">
+      <c r="V16" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>132</v>
       </c>
       <c r="B17" t="s">
+        <v>272</v>
+      </c>
+      <c r="C17" t="s">
+        <v>291</v>
+      </c>
+      <c r="D17" t="s">
         <v>58</v>
       </c>
-      <c r="C17" t="s">
+      <c r="E17" t="s">
         <v>22</v>
       </c>
-      <c r="D17" t="s">
+      <c r="F17" t="s">
         <v>23</v>
       </c>
-      <c r="E17" t="s">
+      <c r="G17" t="s">
         <v>24</v>
       </c>
-      <c r="F17" t="s">
+      <c r="H17" t="s">
         <v>52</v>
       </c>
-      <c r="G17" t="s">
-        <v>30</v>
-      </c>
-      <c r="H17" t="s">
+      <c r="I17" t="s">
+        <v>30</v>
+      </c>
+      <c r="J17" t="s">
         <v>53</v>
       </c>
-      <c r="I17" t="s">
+      <c r="K17" t="s">
         <v>28</v>
       </c>
-      <c r="J17" t="s">
+      <c r="L17" t="s">
         <v>133</v>
       </c>
-      <c r="K17" t="s">
+      <c r="M17" t="s">
         <v>251</v>
       </c>
-      <c r="L17" t="s">
+      <c r="N17" t="s">
         <v>233</v>
       </c>
-      <c r="N17" t="s">
+      <c r="P17" t="s">
         <v>199</v>
       </c>
-      <c r="O17" t="s">
+      <c r="Q17" t="s">
         <v>177</v>
       </c>
-      <c r="P17" t="s">
+      <c r="R17" t="s">
         <v>163</v>
       </c>
-      <c r="Q17" t="s">
+      <c r="S17" t="s">
         <v>134</v>
       </c>
-      <c r="R17" t="s">
+      <c r="T17" t="s">
         <v>135</v>
       </c>
-      <c r="S17" t="s">
+      <c r="U17" t="s">
         <v>136</v>
       </c>
-      <c r="T17" t="s">
+      <c r="V17" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>137</v>
       </c>
       <c r="B18" t="s">
+        <v>273</v>
+      </c>
+      <c r="C18" t="s">
+        <v>292</v>
+      </c>
+      <c r="D18" t="s">
         <v>58</v>
       </c>
-      <c r="C18" t="s">
+      <c r="E18" t="s">
         <v>112</v>
       </c>
-      <c r="D18" t="s">
+      <c r="F18" t="s">
         <v>79</v>
       </c>
-      <c r="E18" t="s">
+      <c r="G18" t="s">
         <v>24</v>
       </c>
-      <c r="F18" t="s">
+      <c r="H18" t="s">
         <v>52</v>
       </c>
-      <c r="G18" t="s">
-        <v>30</v>
-      </c>
-      <c r="H18" t="s">
+      <c r="I18" t="s">
+        <v>30</v>
+      </c>
+      <c r="J18" t="s">
         <v>108</v>
       </c>
-      <c r="I18" t="s">
+      <c r="K18" t="s">
         <v>28</v>
       </c>
-      <c r="J18" t="s">
+      <c r="L18" t="s">
         <v>138</v>
       </c>
-      <c r="K18" t="s">
+      <c r="M18" t="s">
         <v>252</v>
       </c>
-      <c r="L18" t="s">
+      <c r="N18" t="s">
         <v>234</v>
       </c>
-      <c r="M18" t="s">
+      <c r="O18" t="s">
         <v>216</v>
       </c>
-      <c r="N18" t="s">
+      <c r="P18" t="s">
         <v>200</v>
       </c>
-      <c r="P18" t="s">
+      <c r="R18" t="s">
         <v>164</v>
       </c>
-      <c r="Q18" t="s">
+      <c r="S18" t="s">
         <v>139</v>
       </c>
-      <c r="R18" t="s">
+      <c r="T18" t="s">
         <v>140</v>
       </c>
-      <c r="S18" t="s">
+      <c r="U18" t="s">
         <v>141</v>
       </c>
-      <c r="T18" t="s">
+      <c r="V18" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>30</v>
       </c>
       <c r="B19" t="s">
+        <v>274</v>
+      </c>
+      <c r="C19" t="s">
+        <v>293</v>
+      </c>
+      <c r="D19" t="s">
         <v>142</v>
       </c>
-      <c r="C19" t="s">
+      <c r="E19" t="s">
         <v>22</v>
       </c>
-      <c r="D19" t="s">
-        <v>30</v>
-      </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
+        <v>30</v>
+      </c>
+      <c r="G19" t="s">
         <v>24</v>
       </c>
-      <c r="F19" t="s">
-        <v>30</v>
-      </c>
-      <c r="G19" t="s">
-        <v>30</v>
-      </c>
       <c r="H19" t="s">
         <v>30</v>
       </c>
@@ -2346,16 +2576,16 @@
         <v>30</v>
       </c>
       <c r="J19" t="s">
+        <v>30</v>
+      </c>
+      <c r="K19" t="s">
+        <v>30</v>
+      </c>
+      <c r="L19" t="s">
         <v>143</v>
       </c>
-      <c r="K19" t="s">
+      <c r="M19" t="s">
         <v>253</v>
-      </c>
-      <c r="L19" t="s">
-        <v>182</v>
-      </c>
-      <c r="M19" t="s">
-        <v>182</v>
       </c>
       <c r="N19" t="s">
         <v>182</v>
@@ -2364,92 +2594,99 @@
         <v>182</v>
       </c>
       <c r="P19" t="s">
+        <v>182</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>182</v>
+      </c>
+      <c r="R19" t="s">
         <v>167</v>
-      </c>
-      <c r="Q19" t="s">
-        <v>144</v>
-      </c>
-      <c r="R19" t="s">
-        <v>144</v>
       </c>
       <c r="S19" t="s">
         <v>144</v>
       </c>
       <c r="T19" t="s">
+        <v>144</v>
+      </c>
+      <c r="U19" t="s">
+        <v>144</v>
+      </c>
+      <c r="V19" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>30</v>
       </c>
       <c r="B20" t="s">
+        <v>275</v>
+      </c>
+      <c r="C20" t="s">
+        <v>294</v>
+      </c>
+      <c r="D20" t="s">
         <v>35</v>
       </c>
-      <c r="C20" t="s">
+      <c r="E20" t="s">
         <v>22</v>
       </c>
-      <c r="D20" t="s">
+      <c r="F20" t="s">
         <v>23</v>
       </c>
-      <c r="E20" t="s">
+      <c r="G20" t="s">
         <v>24</v>
       </c>
-      <c r="F20" t="s">
+      <c r="H20" t="s">
         <v>52</v>
       </c>
-      <c r="G20" t="s">
-        <v>30</v>
-      </c>
-      <c r="H20" t="s">
+      <c r="I20" t="s">
+        <v>30</v>
+      </c>
+      <c r="J20" t="s">
         <v>145</v>
       </c>
-      <c r="I20" t="s">
+      <c r="K20" t="s">
         <v>28</v>
       </c>
-      <c r="J20" t="s">
+      <c r="L20" t="s">
         <v>146</v>
       </c>
-      <c r="K20" t="s">
+      <c r="M20" t="s">
         <v>254</v>
       </c>
-      <c r="L20" t="s">
+      <c r="N20" t="s">
         <v>235</v>
       </c>
-      <c r="M20" t="s">
+      <c r="O20" t="s">
         <v>217</v>
       </c>
-      <c r="N20" t="s">
+      <c r="P20" t="s">
         <v>201</v>
       </c>
-      <c r="O20" t="s">
+      <c r="Q20" t="s">
         <v>178</v>
       </c>
-      <c r="P20" t="s">
+      <c r="R20" t="s">
         <v>165</v>
       </c>
-      <c r="Q20" t="s">
+      <c r="S20" t="s">
         <v>147</v>
       </c>
-      <c r="R20" t="s">
+      <c r="T20" t="s">
         <v>148</v>
       </c>
-      <c r="S20" t="s">
+      <c r="U20" t="s">
         <v>149</v>
       </c>
-      <c r="T20" t="s">
+      <c r="V20" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:20" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="1:20" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="1:20" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:20" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:20" ht="15.75" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:T1 A20:J20 Q2:T20 A2:J19" numberStoredAsText="1"/>
+    <ignoredError sqref="D1:V1 D20:L20 S2:V20 D2:L19 A2:A19 A20 A1" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>